<commit_message>
- Added and updated documentation
</commit_message>
<xml_diff>
--- a/Documentation/GanttChart.xlsx
+++ b/Documentation/GanttChart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hayden 1/Desktop/School/AIT/AIT Website Task/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hayden\Desktop\AIT-TravelWebsite\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9777FBEB-2725-4D71-A965-2F71E476CB59}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -231,8 +232,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -586,6 +587,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -634,32 +641,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
-    <cellStyle name="Actual legend" xfId="15"/>
+    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Label" xfId="5"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Period Value" xfId="13"/>
-    <cellStyle name="Plan legend" xfId="14"/>
-    <cellStyle name="Project Headers" xfId="4"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
@@ -1044,8 +1045,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1055,35 +1056,35 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="44.6640625" style="2" customWidth="1"/>
-    <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.6640625" style="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="44.625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" style="4" customWidth="1"/>
+    <col min="8" max="27" width="2.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1">
+      <c r="B1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-    </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+    </row>
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="5" t="s">
         <v>25</v>
       </c>
@@ -1091,66 +1092,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="32"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="28" t="s">
+      <c r="Q2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="30"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="32"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="20" t="s">
+      <c r="V2" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="32"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="34"/>
       <c r="Z2" s="17"/>
-      <c r="AA2" s="33" t="s">
+      <c r="AA2" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="35"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="37"/>
       <c r="AH2" s="18"/>
-      <c r="AI2" s="20" t="s">
+      <c r="AI2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AL2" s="21"/>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="21"/>
-      <c r="AO2" s="21"/>
-      <c r="AP2" s="21"/>
-    </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="23" t="s">
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
+    </row>
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
+      <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="29" t="s">
         <v>30</v>
       </c>
       <c r="H3" s="19" t="s">
@@ -1176,13 +1177,13 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1">
+      <c r="B4" s="26"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1364,7 +1365,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:67" ht="30" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:67" ht="30" customHeight="1">
       <c r="B6" s="6" t="s">
         <v>36</v>
       </c>
@@ -1404,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:67" ht="30" customHeight="1">
       <c r="B7" s="6" t="s">
         <v>37</v>
       </c>
@@ -1424,7 +1425,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:67" ht="30" customHeight="1">
       <c r="B8" s="6" t="s">
         <v>38</v>
       </c>
@@ -1444,7 +1445,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:67" ht="30" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>39</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:67" ht="30" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="7">
         <v>4</v>
@@ -1482,7 +1483,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:67" ht="30" customHeight="1">
       <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:67" ht="30" customHeight="1">
       <c r="B12" s="6" t="s">
         <v>3</v>
       </c>
@@ -1522,7 +1523,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:67" ht="30" customHeight="1">
       <c r="B13" s="6" t="s">
         <v>4</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:67" ht="30" customHeight="1">
       <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
@@ -1562,7 +1563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:67" ht="30" customHeight="1">
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
@@ -1582,7 +1583,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:67" ht="30" customHeight="1">
       <c r="B16" s="6" t="s">
         <v>7</v>
       </c>
@@ -1602,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="30" customHeight="1">
       <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
@@ -1622,7 +1623,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="30" customHeight="1">
       <c r="B18" s="6" t="s">
         <v>9</v>
       </c>
@@ -1642,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="30" customHeight="1">
       <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="30" customHeight="1">
       <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1682,7 +1683,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="30" customHeight="1">
       <c r="B21" s="6" t="s">
         <v>12</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="30" customHeight="1">
       <c r="B22" s="6" t="s">
         <v>13</v>
       </c>
@@ -1722,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="30" customHeight="1">
       <c r="B23" s="6" t="s">
         <v>14</v>
       </c>
@@ -1742,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="30" customHeight="1">
       <c r="B24" s="6" t="s">
         <v>15</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="30" customHeight="1">
       <c r="B25" s="6" t="s">
         <v>16</v>
       </c>
@@ -1782,7 +1783,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" ht="30" customHeight="1">
       <c r="B26" s="6" t="s">
         <v>17</v>
       </c>
@@ -1802,7 +1803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" ht="30" customHeight="1">
       <c r="B27" s="6" t="s">
         <v>18</v>
       </c>
@@ -1822,7 +1823,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" ht="30" customHeight="1">
       <c r="B28" s="6" t="s">
         <v>19</v>
       </c>
@@ -1842,7 +1843,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" ht="30" customHeight="1">
       <c r="B29" s="6" t="s">
         <v>20</v>
       </c>
@@ -1862,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" ht="30" customHeight="1">
       <c r="B30" s="6" t="s">
         <v>21</v>
       </c>
@@ -1935,24 +1936,24 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>